<commit_message>
Update spreadsheet sample file in sample files dir
</commit_message>
<xml_diff>
--- a/sample files/spreadsheet_import_sample.xlsx
+++ b/sample files/spreadsheet_import_sample.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EECDA5-BEF8-C547-94A2-37588DCC5648}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19147" windowHeight="9585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CF Doc" sheetId="1" r:id="rId1"/>
     <sheet name="CF Item" sheetId="2" r:id="rId2"/>
     <sheet name="CF Association" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
   <si>
     <t>identifier</t>
   </si>
@@ -72,6 +66,24 @@
     <t>notes</t>
   </si>
   <si>
+    <t>93a2d99e-2988-11e9-8a65-bf64185a38dc</t>
+  </si>
+  <si>
+    <t>ImportSpreadsheet</t>
+  </si>
+  <si>
+    <t>SampleFramework</t>
+  </si>
+  <si>
+    <t>2019-02-05 20:56:58</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>2019-02-05 00:00:00</t>
+  </si>
+  <si>
     <t>fullStatement</t>
   </si>
   <si>
@@ -99,6 +111,72 @@
     <t>license</t>
   </si>
   <si>
+    <t>statement</t>
+  </si>
+  <si>
+    <t>93a2f014-2988-11e9-a3f0-673da56e176f</t>
+  </si>
+  <si>
+    <t>Statement 1</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>93a34668-2988-11e9-b303-4d039254c617</t>
+  </si>
+  <si>
+    <t>Statement 2</t>
+  </si>
+  <si>
+    <t>S.1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>Major Strand</t>
+  </si>
+  <si>
+    <t>93a38c04-2988-11e9-965c-13cdc43414be</t>
+  </si>
+  <si>
+    <t>Statement 3</t>
+  </si>
+  <si>
+    <t>S.2</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>93a3ccbe-2988-11e9-9e42-cd0bdac30e98</t>
+  </si>
+  <si>
+    <t>Statement 4</t>
+  </si>
+  <si>
+    <t>S.2.1</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>Child Statement</t>
+  </si>
+  <si>
     <t>originNodeIdentifier</t>
   </si>
   <si>
@@ -120,77 +198,430 @@
     <t>associationGroupName</t>
   </si>
   <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>Statement 1</t>
-  </si>
-  <si>
-    <t>Statement 2</t>
-  </si>
-  <si>
-    <t>Statement 3</t>
-  </si>
-  <si>
-    <t>Statement 4</t>
-  </si>
-  <si>
-    <t>S.1</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>S.2</t>
-  </si>
-  <si>
-    <t>S.2.1</t>
-  </si>
-  <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>Cluster</t>
-  </si>
-  <si>
-    <t>Major Strand</t>
-  </si>
-  <si>
-    <t>Statement</t>
-  </si>
-  <si>
-    <t>Child Statement</t>
-  </si>
-  <si>
-    <t>ImportSpreadsheet</t>
-  </si>
-  <si>
-    <t>SampleFramework</t>
+    <t>93a4925c-2988-11e9-be52-5daeaa7fb2e9</t>
+  </si>
+  <si>
+    <t>Is Child Of</t>
+  </si>
+  <si>
+    <t>93a49478-2988-11e9-b4e9-477f7e3210b8</t>
+  </si>
+  <si>
+    <t>93a495e0-2988-11e9-b442-21f50a619a7c</t>
+  </si>
+  <si>
+    <t>93a4975c-2988-11e9-bc71-531ae09cd3b7</t>
+  </si>
+  <si>
+    <t>b0b46020-2988-11e9-be1a-7f1a067737d4</t>
+  </si>
+  <si>
+    <t>Exact Match Of</t>
+  </si>
+  <si>
+    <t>9ce35718-abcf-11e8-82fc-3933f2f03ee8</t>
+  </si>
+  <si>
+    <t>b3bac9da-2988-11e9-89ec-a7ed6f798df9</t>
+  </si>
+  <si>
+    <t>Is Part Of</t>
+  </si>
+  <si>
+    <t>b5ba2d5c-2988-11e9-bb44-bb2cafbe3ae5</t>
+  </si>
+  <si>
+    <t>Precedes</t>
+  </si>
+  <si>
+    <t>71d0bd26-abd0-11e8-bee4-1349da53c60c</t>
+  </si>
+  <si>
+    <t>b8cb5160-2988-11e9-922f-ffe8c1749b01</t>
+  </si>
+  <si>
+    <t>Replaced By</t>
+  </si>
+  <si>
+    <t>bc790afa-2988-11e9-a61c-69bffc17d8fd</t>
+  </si>
+  <si>
+    <t>Human.Coding</t>
+  </si>
+  <si>
+    <t>Has Skill Level</t>
+  </si>
+  <si>
+    <t>beff57f2-2988-11e9-8897-637ca06a980b</t>
+  </si>
+  <si>
+    <t>Is Peer Of</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -198,32 +629,309 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -232,7 +940,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -513,16 +1221,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <cols>
+    <col min="2" max="2" width="17.96" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,58 +1284,69 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="8.83203125" style="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
@@ -632,126 +1355,314 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="K2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
       <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.2</v>
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
       </c>
       <c r="J4">
         <v>6</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="7"/>
+  <cols>
+    <col min="4" max="4" width="33.9466666666667" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>